<commit_message>
alteração dos diagramas, implementação do modelo ABNT no documento e inserção de tópicos
</commit_message>
<xml_diff>
--- a/documentacao/cronograma_ABNT_2020_PTCC - REF.xlsx
+++ b/documentacao/cronograma_ABNT_2020_PTCC - REF.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Mestre\Downloads\PTCC\PTCC02_-_Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TCC\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{4C4C6232-E017-CA46-B294-C0DED9FDD640}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CDB35C94-BF83-4499-A92E-3812B002D9F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7505BF7E-3EF0-4DC8-8E83-7AC43EA79C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="complete schedule " sheetId="1" r:id="rId1"/>
+    <sheet name="schedule part1" sheetId="4" r:id="rId2"/>
+    <sheet name="schedule part2" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t>Meses
 X
@@ -71,9 +70,6 @@
   </si>
   <si>
     <t>Junho</t>
-  </si>
-  <si>
-    <t>Julho</t>
   </si>
   <si>
     <t>Estudo do cenário da área profissional.</t>
@@ -139,26 +135,26 @@
     <t>Desenvolvimento do Web Site com Html, Css e Boostrap</t>
   </si>
   <si>
-    <t>Criação e implementação do Banco de dados no Projeto  com o uso de PHP e Heroku</t>
-  </si>
-  <si>
     <t>Desenvolvimento da usabilidade do Web Site com Java Script</t>
   </si>
   <si>
-    <t>Correção de possiveis erros e refatoração do projeto</t>
+    <t>Apresentação e entrega do TCC</t>
   </si>
   <si>
-    <t>Criação de documentação para apresentação do Projeto Final</t>
+    <t>Preparativos para apresentação do Projeto Final</t>
   </si>
   <si>
-    <t>Apresentação e entrega do TCC</t>
+    <t>Criação e implementação do Banco de dados no Projeto</t>
+  </si>
+  <si>
+    <t>Refatoração do projeto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -332,12 +328,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -375,15 +395,26 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -404,7 +435,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -729,100 +760,99 @@
   </sheetPr>
   <dimension ref="A2:BA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A15" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41.42578125" customWidth="1"/>
     <col min="3" max="49" width="1.7109375" customWidth="1"/>
     <col min="50" max="52" width="1.5703125" customWidth="1"/>
+    <col min="54" max="54" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:49" ht="60" customHeight="1">
+    <row r="3" spans="1:49" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25" t="s">
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25" t="s">
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25" t="s">
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25" t="s">
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25" t="s">
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25" t="s">
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25" t="s">
+      <c r="AI3" s="32"/>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25" t="s">
+      <c r="AM3" s="32"/>
+      <c r="AN3" s="32"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25" t="s">
+      <c r="AQ3" s="32"/>
+      <c r="AR3" s="32"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="30"/>
+      <c r="AU3" s="30"/>
+      <c r="AV3" s="30"/>
+      <c r="AW3" s="30"/>
+    </row>
+    <row r="4" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="AU3" s="25"/>
-      <c r="AV3" s="25"/>
-      <c r="AW3" s="25"/>
-    </row>
-    <row r="4" spans="1:49" ht="21.95" customHeight="1">
-      <c r="B4" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -867,14 +897,14 @@
       <c r="AQ4" s="1"/>
       <c r="AR4" s="2"/>
       <c r="AS4" s="1"/>
-      <c r="AT4" s="2"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="2"/>
-      <c r="AW4" s="1"/>
-    </row>
-    <row r="5" spans="1:49" ht="33" customHeight="1">
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="28"/>
+      <c r="AW4" s="9"/>
+    </row>
+    <row r="5" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -919,14 +949,14 @@
       <c r="AQ5" s="1"/>
       <c r="AR5" s="2"/>
       <c r="AS5" s="1"/>
-      <c r="AT5" s="2"/>
-      <c r="AU5" s="1"/>
-      <c r="AV5" s="2"/>
-      <c r="AW5" s="1"/>
-    </row>
-    <row r="6" spans="1:49" ht="21.95" customHeight="1">
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="9"/>
+    </row>
+    <row r="6" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -971,14 +1001,10 @@
       <c r="AQ6" s="6"/>
       <c r="AR6" s="5"/>
       <c r="AS6" s="6"/>
-      <c r="AT6" s="5"/>
-      <c r="AU6" s="6"/>
-      <c r="AV6" s="5"/>
-      <c r="AW6" s="6"/>
-    </row>
-    <row r="7" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="7" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1023,14 +1049,10 @@
       <c r="AQ7" s="6"/>
       <c r="AR7" s="5"/>
       <c r="AS7" s="6"/>
-      <c r="AT7" s="5"/>
-      <c r="AU7" s="6"/>
-      <c r="AV7" s="5"/>
-      <c r="AW7" s="6"/>
-    </row>
-    <row r="8" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="8" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1075,14 +1097,10 @@
       <c r="AQ8" s="6"/>
       <c r="AR8" s="5"/>
       <c r="AS8" s="6"/>
-      <c r="AT8" s="5"/>
-      <c r="AU8" s="6"/>
-      <c r="AV8" s="5"/>
-      <c r="AW8" s="6"/>
-    </row>
-    <row r="9" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="9" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1127,14 +1145,10 @@
       <c r="AQ9" s="6"/>
       <c r="AR9" s="5"/>
       <c r="AS9" s="6"/>
-      <c r="AT9" s="5"/>
-      <c r="AU9" s="6"/>
-      <c r="AV9" s="5"/>
-      <c r="AW9" s="6"/>
-    </row>
-    <row r="10" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="10" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1179,14 +1193,10 @@
       <c r="AQ10" s="6"/>
       <c r="AR10" s="5"/>
       <c r="AS10" s="6"/>
-      <c r="AT10" s="5"/>
-      <c r="AU10" s="6"/>
-      <c r="AV10" s="5"/>
-      <c r="AW10" s="6"/>
-    </row>
-    <row r="11" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="11" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1231,14 +1241,10 @@
       <c r="AQ11" s="6"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="6"/>
-      <c r="AT11" s="5"/>
-      <c r="AU11" s="6"/>
-      <c r="AV11" s="5"/>
-      <c r="AW11" s="6"/>
-    </row>
-    <row r="12" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="12" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -1283,14 +1289,10 @@
       <c r="AQ12" s="6"/>
       <c r="AR12" s="5"/>
       <c r="AS12" s="6"/>
-      <c r="AT12" s="5"/>
-      <c r="AU12" s="6"/>
-      <c r="AV12" s="5"/>
-      <c r="AW12" s="6"/>
-    </row>
-    <row r="13" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="13" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1335,14 +1337,10 @@
       <c r="AQ13" s="6"/>
       <c r="AR13" s="5"/>
       <c r="AS13" s="6"/>
-      <c r="AT13" s="5"/>
-      <c r="AU13" s="6"/>
-      <c r="AV13" s="5"/>
-      <c r="AW13" s="6"/>
-    </row>
-    <row r="14" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="14" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="5"/>
@@ -1387,14 +1385,10 @@
       <c r="AQ14" s="6"/>
       <c r="AR14" s="5"/>
       <c r="AS14" s="6"/>
-      <c r="AT14" s="5"/>
-      <c r="AU14" s="6"/>
-      <c r="AV14" s="5"/>
-      <c r="AW14" s="6"/>
-    </row>
-    <row r="15" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="15" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1439,14 +1433,10 @@
       <c r="AQ15" s="6"/>
       <c r="AR15" s="5"/>
       <c r="AS15" s="6"/>
-      <c r="AT15" s="5"/>
-      <c r="AU15" s="6"/>
-      <c r="AV15" s="5"/>
-      <c r="AW15" s="6"/>
-    </row>
-    <row r="16" spans="1:49" ht="21.95" customHeight="1">
+    </row>
+    <row r="16" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="12"/>
@@ -1491,14 +1481,10 @@
       <c r="AQ16" s="6"/>
       <c r="AR16" s="5"/>
       <c r="AS16" s="6"/>
-      <c r="AT16" s="5"/>
-      <c r="AU16" s="6"/>
-      <c r="AV16" s="5"/>
-      <c r="AW16" s="6"/>
-    </row>
-    <row r="17" spans="2:53" ht="21.95" customHeight="1">
+    </row>
+    <row r="17" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="19"/>
@@ -1539,18 +1525,14 @@
       <c r="AM17" s="13"/>
       <c r="AN17" s="12"/>
       <c r="AO17" s="13"/>
-      <c r="AP17" s="12"/>
-      <c r="AQ17" s="13"/>
-      <c r="AR17" s="12"/>
-      <c r="AS17" s="13"/>
-      <c r="AT17" s="12"/>
-      <c r="AU17" s="13"/>
-      <c r="AV17" s="12"/>
-      <c r="AW17" s="13"/>
-    </row>
-    <row r="18" spans="2:53" ht="21.95" customHeight="1">
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="6"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="6"/>
+    </row>
+    <row r="18" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1591,18 +1573,14 @@
       <c r="AM18" s="6"/>
       <c r="AN18" s="16"/>
       <c r="AO18" s="6"/>
-      <c r="AP18" s="16"/>
+      <c r="AP18" s="6"/>
       <c r="AQ18" s="6"/>
-      <c r="AR18" s="16"/>
+      <c r="AR18" s="6"/>
       <c r="AS18" s="6"/>
-      <c r="AT18" s="16"/>
-      <c r="AU18" s="6"/>
-      <c r="AV18" s="16"/>
-      <c r="AW18" s="6"/>
-    </row>
-    <row r="19" spans="2:53" ht="21.95" customHeight="1">
+    </row>
+    <row r="19" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -1643,18 +1621,14 @@
       <c r="AM19" s="6"/>
       <c r="AN19" s="14"/>
       <c r="AO19" s="6"/>
-      <c r="AP19" s="14"/>
+      <c r="AP19" s="6"/>
       <c r="AQ19" s="6"/>
-      <c r="AR19" s="14"/>
+      <c r="AR19" s="6"/>
       <c r="AS19" s="6"/>
-      <c r="AT19" s="14"/>
-      <c r="AU19" s="6"/>
-      <c r="AV19" s="14"/>
-      <c r="AW19" s="6"/>
-    </row>
-    <row r="20" spans="2:53" ht="21.95" customHeight="1">
+    </row>
+    <row r="20" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1699,14 +1673,10 @@
       <c r="AQ20" s="6"/>
       <c r="AR20" s="6"/>
       <c r="AS20" s="6"/>
-      <c r="AT20" s="6"/>
-      <c r="AU20" s="6"/>
-      <c r="AV20" s="6"/>
-      <c r="AW20" s="6"/>
-    </row>
-    <row r="21" spans="2:53" ht="21.95" customHeight="1">
+    </row>
+    <row r="21" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="6"/>
@@ -1751,14 +1721,10 @@
       <c r="AQ21" s="6"/>
       <c r="AR21" s="6"/>
       <c r="AS21" s="6"/>
-      <c r="AT21" s="6"/>
-      <c r="AU21" s="6"/>
-      <c r="AV21" s="6"/>
-      <c r="AW21" s="6"/>
-    </row>
-    <row r="22" spans="2:53" ht="21.95" customHeight="1">
+    </row>
+    <row r="22" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1803,14 +1769,10 @@
       <c r="AQ22" s="6"/>
       <c r="AR22" s="6"/>
       <c r="AS22" s="6"/>
-      <c r="AT22" s="6"/>
-      <c r="AU22" s="6"/>
-      <c r="AV22" s="6"/>
-      <c r="AW22" s="6"/>
-    </row>
-    <row r="23" spans="2:53" ht="20.25" customHeight="1">
-      <c r="B23" s="26" t="s">
-        <v>31</v>
+    </row>
+    <row r="23" spans="2:53" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
+        <v>30</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1855,14 +1817,10 @@
       <c r="AQ23" s="6"/>
       <c r="AR23" s="6"/>
       <c r="AS23" s="5"/>
-      <c r="AT23" s="5"/>
-      <c r="AU23" s="6"/>
-      <c r="AV23" s="6"/>
-      <c r="AW23" s="6"/>
-    </row>
-    <row r="24" spans="2:53" ht="30.75" customHeight="1">
+    </row>
+    <row r="24" spans="2:53" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1907,14 +1865,10 @@
       <c r="AQ24" s="6"/>
       <c r="AR24" s="6"/>
       <c r="AS24" s="5"/>
-      <c r="AT24" s="5"/>
-      <c r="AU24" s="6"/>
-      <c r="AV24" s="6"/>
-      <c r="AW24" s="6"/>
-    </row>
-    <row r="25" spans="2:53" ht="31.5" customHeight="1">
+    </row>
+    <row r="25" spans="2:53" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1959,14 +1913,10 @@
       <c r="AQ25" s="6"/>
       <c r="AR25" s="6"/>
       <c r="AS25" s="6"/>
-      <c r="AT25" s="5"/>
-      <c r="AU25" s="6"/>
-      <c r="AV25" s="6"/>
-      <c r="AW25" s="6"/>
-    </row>
-    <row r="26" spans="2:53" ht="28.5" customHeight="1">
+    </row>
+    <row r="26" spans="2:53" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -2011,14 +1961,10 @@
       <c r="AQ26" s="6"/>
       <c r="AR26" s="6"/>
       <c r="AS26" s="6"/>
-      <c r="AT26" s="5"/>
-      <c r="AU26" s="6"/>
-      <c r="AV26" s="6"/>
-      <c r="AW26" s="6"/>
-    </row>
-    <row r="27" spans="2:53" ht="33" customHeight="1">
+    </row>
+    <row r="27" spans="2:53" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -2063,14 +2009,10 @@
       <c r="AQ27" s="6"/>
       <c r="AR27" s="6"/>
       <c r="AS27" s="6"/>
-      <c r="AT27" s="5"/>
-      <c r="AU27" s="6"/>
-      <c r="AV27" s="6"/>
-      <c r="AW27" s="6"/>
-    </row>
-    <row r="28" spans="2:53" ht="24" customHeight="1">
+    </row>
+    <row r="28" spans="2:53" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -2111,19 +2053,15 @@
       <c r="AM28" s="6"/>
       <c r="AN28" s="6"/>
       <c r="AO28" s="6"/>
-      <c r="AP28" s="24"/>
-      <c r="AQ28" s="24"/>
+      <c r="AP28" s="19"/>
+      <c r="AQ28" s="19"/>
       <c r="AR28" s="6"/>
       <c r="AS28" s="6"/>
-      <c r="AT28" s="5"/>
-      <c r="AU28" s="6"/>
-      <c r="AV28" s="6"/>
-      <c r="AW28" s="6"/>
-      <c r="BA28" s="27"/>
-    </row>
-    <row r="29" spans="2:53" ht="31.5" customHeight="1">
+      <c r="BA28" s="26"/>
+    </row>
+    <row r="29" spans="2:53" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -2164,18 +2102,14 @@
       <c r="AM29" s="6"/>
       <c r="AN29" s="6"/>
       <c r="AO29" s="6"/>
-      <c r="AP29" s="24"/>
-      <c r="AQ29" s="24"/>
-      <c r="AR29" s="24"/>
-      <c r="AS29" s="24"/>
-      <c r="AT29" s="5"/>
-      <c r="AU29" s="6"/>
-      <c r="AV29" s="6"/>
-      <c r="AW29" s="6"/>
-    </row>
-    <row r="30" spans="2:53" ht="29.25" customHeight="1">
-      <c r="B30" s="28" t="s">
-        <v>38</v>
+      <c r="AP29" s="19"/>
+      <c r="AQ29" s="19"/>
+      <c r="AR29" s="29"/>
+      <c r="AS29" s="29"/>
+    </row>
+    <row r="30" spans="2:53" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -2218,19 +2152,14 @@
       <c r="AO30" s="6"/>
       <c r="AP30" s="5"/>
       <c r="AQ30" s="6"/>
-      <c r="AR30" s="6"/>
-      <c r="AS30" s="6"/>
-      <c r="AT30" s="24"/>
-      <c r="AU30" s="24"/>
-      <c r="AV30" s="24"/>
-      <c r="AW30" s="24"/>
+      <c r="AR30" s="20"/>
+      <c r="AS30" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="AH3:AK3"/>
     <mergeCell ref="AL3:AO3"/>
     <mergeCell ref="AP3:AS3"/>
-    <mergeCell ref="AT3:AW3"/>
     <mergeCell ref="V3:Y3"/>
     <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="AD3:AG3"/>
@@ -2246,47 +2175,1581 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFB72EE-7B21-4EE8-84D0-418978EC27AC}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:BA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BE9" sqref="BE9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="49" width="1.7109375" customWidth="1"/>
+    <col min="50" max="52" width="1.5703125" customWidth="1"/>
+    <col min="54" max="54" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:49" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI3" s="32"/>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="32"/>
+      <c r="AN3" s="32"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ3" s="32"/>
+      <c r="AR3" s="32"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="30"/>
+      <c r="AU3" s="30"/>
+      <c r="AV3" s="30"/>
+      <c r="AW3" s="30"/>
+    </row>
+    <row r="4" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="28"/>
+      <c r="AW4" s="9"/>
+    </row>
+    <row r="5" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="9"/>
+    </row>
+    <row r="6" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="6"/>
+    </row>
+    <row r="7" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="5"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="5"/>
+      <c r="AS7" s="6"/>
+    </row>
+    <row r="8" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="5"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="5"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="5"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="5"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="5"/>
+      <c r="AS8" s="6"/>
+    </row>
+    <row r="9" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="5"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="5"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="5"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="5"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="5"/>
+      <c r="AS9" s="6"/>
+    </row>
+    <row r="10" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="5"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="5"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="5"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="5"/>
+      <c r="AS10" s="6"/>
+    </row>
+    <row r="11" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="5"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="6"/>
+      <c r="AL11" s="5"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="5"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="5"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="5"/>
+      <c r="AS11" s="6"/>
+    </row>
+    <row r="12" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="5"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="5"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="5"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="6"/>
+      <c r="AR12" s="5"/>
+      <c r="AS12" s="6"/>
+    </row>
+    <row r="13" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="6"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="6"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="6"/>
+    </row>
+    <row r="14" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="5"/>
+      <c r="AQ14" s="6"/>
+      <c r="AR14" s="5"/>
+      <c r="AS14" s="6"/>
+    </row>
+    <row r="15" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="5"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="5"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="5"/>
+      <c r="AM15" s="6"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="6"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="6"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="6"/>
+    </row>
+    <row r="16" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="5"/>
+      <c r="AK16" s="6"/>
+      <c r="AL16" s="5"/>
+      <c r="AM16" s="6"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="6"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="6"/>
+      <c r="AR16" s="5"/>
+      <c r="AS16" s="6"/>
+    </row>
+    <row r="17" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="5"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="5"/>
+      <c r="AK17" s="6"/>
+      <c r="AL17" s="5"/>
+      <c r="AM17" s="6"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="6"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="6"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="6"/>
+    </row>
+    <row r="18" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:53" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:53" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:53" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:53" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:53" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:53" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BA28" s="26"/>
+    </row>
+    <row r="29" spans="2:53" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:53" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AP3:AS3"/>
+  </mergeCells>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="79" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF23FF2-9280-4C07-A182-DC2E7E28E857}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:BA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BF10" sqref="BF10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="49" width="1.7109375" customWidth="1"/>
+    <col min="50" max="52" width="1.5703125" customWidth="1"/>
+    <col min="54" max="54" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:49" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="32"/>
+      <c r="AF3" s="32"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI3" s="32"/>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM3" s="32"/>
+      <c r="AN3" s="32"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ3" s="32"/>
+      <c r="AR3" s="32"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="30"/>
+      <c r="AU3" s="30"/>
+      <c r="AV3" s="30"/>
+      <c r="AW3" s="30"/>
+    </row>
+    <row r="4" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="16"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="16"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="28"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="28"/>
+      <c r="AW4" s="9"/>
+    </row>
+    <row r="5" spans="1:49" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="28"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="9"/>
+    </row>
+    <row r="6" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="6"/>
+      <c r="AS6" s="6"/>
+    </row>
+    <row r="7" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+    </row>
+    <row r="8" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="6"/>
+    </row>
+    <row r="9" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="5"/>
+      <c r="AH9" s="5"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="5"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="5"/>
+      <c r="AP9" s="5"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="5"/>
+    </row>
+    <row r="10" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="5"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="5"/>
+      <c r="AP10" s="5"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="5"/>
+    </row>
+    <row r="11" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="5"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="5"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+    </row>
+    <row r="12" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="19"/>
+      <c r="AI12" s="19"/>
+      <c r="AJ12" s="24"/>
+      <c r="AK12" s="24"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="6"/>
+      <c r="AO12" s="6"/>
+      <c r="AP12" s="5"/>
+      <c r="AQ12" s="6"/>
+      <c r="AR12" s="6"/>
+      <c r="AS12" s="6"/>
+    </row>
+    <row r="13" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="19"/>
+      <c r="AI13" s="19"/>
+      <c r="AJ13" s="24"/>
+      <c r="AK13" s="24"/>
+      <c r="AL13" s="19"/>
+      <c r="AM13" s="19"/>
+      <c r="AN13" s="24"/>
+      <c r="AO13" s="24"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="6"/>
+      <c r="AR13" s="6"/>
+      <c r="AS13" s="6"/>
+    </row>
+    <row r="14" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="19"/>
+      <c r="AQ14" s="19"/>
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
+    </row>
+    <row r="15" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="6"/>
+      <c r="AN15" s="6"/>
+      <c r="AO15" s="6"/>
+      <c r="AP15" s="19"/>
+      <c r="AQ15" s="19"/>
+      <c r="AR15" s="29"/>
+      <c r="AS15" s="29"/>
+    </row>
+    <row r="16" spans="1:49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="6"/>
+      <c r="AK16" s="6"/>
+      <c r="AL16" s="6"/>
+      <c r="AM16" s="6"/>
+      <c r="AN16" s="6"/>
+      <c r="AO16" s="6"/>
+      <c r="AP16" s="5"/>
+      <c r="AQ16" s="6"/>
+      <c r="AR16" s="20"/>
+      <c r="AS16" s="20"/>
+    </row>
+    <row r="17" spans="53:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="53:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="53:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="53:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="53:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="53:53" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="53:53" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="53:53" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="53:53" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="53:53" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="53:53" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="53:53" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BA28" s="26"/>
+    </row>
+    <row r="29" spans="53:53" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="53:53" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AP3:AS3"/>
+  </mergeCells>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="79" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="edbb474b-5c4d-4d44-b638-4e0c2c7a1687" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006510470ED84D1042AEF92873B0DB06CC" ma:contentTypeVersion="7" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="bbba227efaf596de9c5157f84be25112">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="edbb474b-5c4d-4d44-b638-4e0c2c7a1687" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b2387608d8e9b7c6d63a16b44ddac7b" ns2:_="">
     <xsd:import namespace="edbb474b-5c4d-4d44-b638-4e0c2c7a1687"/>
@@ -2450,14 +3913,55 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="edbb474b-5c4d-4d44-b638-4e0c2c7a1687" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{988438D3-8385-49A2-B3FB-92DA27623D0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5634144D-BF67-4F9E-AED8-E752743FF378}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="edbb474b-5c4d-4d44-b638-4e0c2c7a1687"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DF4CE98-67FD-4540-9A5E-460FC02F8EDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{988438D3-8385-49A2-B3FB-92DA27623D0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="edbb474b-5c4d-4d44-b638-4e0c2c7a1687"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5634144D-BF67-4F9E-AED8-E752743FF378}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DF4CE98-67FD-4540-9A5E-460FC02F8EDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>